<commit_message>
word is correct once
</commit_message>
<xml_diff>
--- a/autoConditions/train1Block1.xlsx
+++ b/autoConditions/train1Block1.xlsx
@@ -449,72 +449,72 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>trainaudio/18_popata.wav</t>
+          <t>trainingaudio/01_kitipi1.wav</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>pngimages/18_donut.png</t>
+          <t>pngimages/01_gift.png</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>trainaudio/27_pakapa.wav</t>
+          <t>trainingaudio/16_kotapi2.wav</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>pngimages/27_kiwi.png</t>
+          <t>pngimages/16_icecream.png</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>trainaudio/10_tokiti.wav</t>
+          <t>trainingaudio/05_titopo2.wav</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>pngimages/100_bicycle.png</t>
+          <t>pngimages/05_megaphone.png</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>trainaudio/22_kakoki.wav</t>
+          <t>trainingaudio/26_kapako1.wav</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>pngimages/22_egg.png</t>
+          <t>pngimages/26_pineapple.png</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>trainaudio/01_kitipi.wav</t>
+          <t>trainingaudio/15_kopota3.wav</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>pngimages/01_gift.png</t>
+          <t>pngimages/15_barrel.png</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>trainaudio/24_takopa.wav</t>
+          <t>trainingaudio/23_patoko1.wav</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>pngimages/24_banana.png</t>
+          <t>pngimages/23_lemon.png</t>
         </is>
       </c>
     </row>

</xml_diff>